<commit_message>
211216 - BLTAnh - Reports
</commit_message>
<xml_diff>
--- a/Docs/Timeline.xlsx
+++ b/Docs/Timeline.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SoftEng\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/19120163_student_hcmus_edu_vn/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D233851-B068-4828-8BB1-F35BB5FA22EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{8249A737-0AAB-4BFA-B6B2-5FB40B02FF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5EC308D-70E7-4FD6-BC66-FB364D37AA87}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +36,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
     <t>Ngày</t>
   </si>
   <si>
@@ -54,80 +60,74 @@
     <t>GOAL</t>
   </si>
   <si>
+    <t>Đăng nhập/Đăng ký</t>
+  </si>
+  <si>
+    <t>Thông tin giải đấu</t>
+  </si>
+  <si>
+    <t>Báo cáo số 3</t>
+  </si>
+  <si>
+    <t>Guest: Xem thông tin giải đấu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User: </t>
+  </si>
+  <si>
+    <t>- Đăng nhập/Đăng ký, lấy thêm thông tin</t>
+  </si>
+  <si>
     <t>Tiền báo cáo 3</t>
   </si>
   <si>
+    <t>- Tạo, tham gia giải đấu (Trừ Hậu cần). Không cần lời mời (Phê duyệt tham gia)</t>
+  </si>
+  <si>
+    <t>Cập nhật trận đấu (HLV, Đội hình ra sân, Bàn thắng, BXH)</t>
+  </si>
+  <si>
+    <t>Tham gia giải đấu</t>
+  </si>
+  <si>
+    <t>Chưa cho phép rời giải đấu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin: </t>
+  </si>
+  <si>
+    <t>- Tạo giải đấu (11 người, bỏ U12, số lượng 8-16, chế độ xem)</t>
+  </si>
+  <si>
+    <t>- Thêm, xem, xoá, sửa giải đấu (khóa một số trường)</t>
+  </si>
+  <si>
+    <t>- Trận đấu: Bàn thắng, đội hình, bảng xếp hạng, kết quả trận đấu</t>
+  </si>
+  <si>
+    <t>- Giải đấu: Cung cấp địa chỉ Email, Facebook, YouTube</t>
+  </si>
+  <si>
     <t>Tiền kiểm chứng</t>
   </si>
   <si>
+    <t>Có giao diện riêng</t>
+  </si>
+  <si>
+    <t>Viết Test-case</t>
+  </si>
+  <si>
+    <t>Tiền mã nguồn</t>
+  </si>
+  <si>
     <t>Nộp mã nguồn</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Guest: Xem thông tin giải đấu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User: </t>
-  </si>
-  <si>
-    <t>- Đăng nhập/Đăng ký, lấy thêm thông tin</t>
-  </si>
-  <si>
-    <t>- Tạo, tham gia giải đấu (Trừ Hậu cần). Không cần lời mời (Phê duyệt tham gia)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin: </t>
-  </si>
-  <si>
-    <t>- Tạo giải đấu (11 người, bỏ U12, số lượng 8-16, chế độ xem)</t>
-  </si>
-  <si>
-    <t>- Thêm, xem, xoá, sửa giải đấu (khóa một số trường)</t>
-  </si>
-  <si>
-    <t>- Trận đấu: Bàn thắng, đội hình, bảng xếp hạng, kết quả trận đấu</t>
-  </si>
-  <si>
-    <t>- Giải đấu: Cung cấp địa chỉ Email, Facebook, YouTube</t>
-  </si>
-  <si>
-    <t>Chưa cho phép rời giải đấu.</t>
-  </si>
-  <si>
-    <t>Có giao diện riêng</t>
-  </si>
-  <si>
-    <t>Đăng nhập/Đăng ký</t>
-  </si>
-  <si>
-    <t>Tham gia giải đấu</t>
-  </si>
-  <si>
-    <t>Cập nhật trận đấu (HLV, Đội hình ra sân, Bàn thắng, BXH)</t>
-  </si>
-  <si>
-    <t>Thông tin giải đấu</t>
-  </si>
-  <si>
-    <t>Báo cáo số 3</t>
-  </si>
-  <si>
-    <t>Viết Test-case</t>
-  </si>
-  <si>
-    <t>Tiền mã nguồn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,8 +151,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +190,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -285,15 +298,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -304,6 +311,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -331,30 +356,25 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -637,285 +657,285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.3984375" customWidth="1"/>
-    <col min="4" max="4" width="23.296875" customWidth="1"/>
+    <col min="4" max="4" width="23.19921875" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="25.796875" customWidth="1"/>
+    <col min="6" max="6" width="25.69921875" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>44532</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="25">
-        <v>44532</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="25">
+      <c r="B5" s="12">
         <v>44533</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="18"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="24"/>
       <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="25">
+      <c r="B6" s="12">
         <v>44534</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="18"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="24"/>
       <c r="I6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="25">
+      <c r="B7" s="12">
         <v>44535</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="19"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="25"/>
       <c r="I7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="26">
+      <c r="B8" s="12">
         <v>44536</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="20" t="s">
-        <v>6</v>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
         <v>44537</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
+        <v>44538</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="24"/>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
+        <v>44539</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="24"/>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
+        <v>44540</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="25"/>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>44541</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="10"/>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
+        <v>44542</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="13"/>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
+        <v>44543</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="17" t="s">
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
+        <v>44544</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="25">
-        <v>44538</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="18"/>
-      <c r="I10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="25">
-        <v>44539</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="18"/>
-      <c r="I11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="25">
-        <v>44540</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="19"/>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="25">
-        <v>44541</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
-      <c r="I13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="25">
-        <v>44542</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="7"/>
-      <c r="I14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="26">
-        <v>44543</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="25">
-        <v>44544</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>44545</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
+        <v>44546</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
+        <v>44547</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>44548</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="25">
-        <v>44545</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="25">
-        <v>44546</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="25">
-        <v>44547</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="25">
-        <v>44548</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="20" t="s">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="7">
+        <v>44549</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="25">
-        <v>44549</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -932,4 +952,246 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100182A0FD1201485479895ED3ABF5F8B85" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="079ee4fb2fabb65520d6a613be97d116">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7b495183-be68-46b6-9f93-303bb4369acc" xmlns:ns4="e8900967-fe10-44ee-8cdd-dcc614f4f1dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="352e32c72f0a7a307122e470dfb98c00" ns3:_="" ns4:_="">
+    <xsd:import namespace="7b495183-be68-46b6-9f93-303bb4369acc"/>
+    <xsd:import namespace="e8900967-fe10-44ee-8cdd-dcc614f4f1dd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7b495183-be68-46b6-9f93-303bb4369acc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e8900967-fe10-44ee-8cdd-dcc614f4f1dd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E70EDAD-331A-46C8-9CBE-243B28A6A96D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1028B10C-001E-4A2B-8DAC-FE067E1C860E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="e8900967-fe10-44ee-8cdd-dcc614f4f1dd"/>
+    <ds:schemaRef ds:uri="7b495183-be68-46b6-9f93-303bb4369acc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E09C09F-8B5A-4369-9A12-6EC610C2EE49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7b495183-be68-46b6-9f93-303bb4369acc"/>
+    <ds:schemaRef ds:uri="e8900967-fe10-44ee-8cdd-dcc614f4f1dd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
220118 - BLTAnh - Change to new organization
</commit_message>
<xml_diff>
--- a/Docs/Timeline.xlsx
+++ b/Docs/Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/19120163_student_hcmus_edu_vn/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SoftEng\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{8249A737-0AAB-4BFA-B6B2-5FB40B02FF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5EC308D-70E7-4FD6-BC66-FB364D37AA87}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C65C7AA-1399-448E-A6B8-F6ECB2CD68EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,18 +180,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -298,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,15 +294,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,40 +302,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,7 +328,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -658,7 +620,7 @@
   <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -681,13 +643,13 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -701,69 +663,69 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>44532</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="23" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="B5" s="8">
         <v>44533</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="24"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="12"/>
       <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
+      <c r="B6" s="8">
         <v>44534</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="24"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="12"/>
       <c r="I6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="8">
         <v>44535</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="13"/>
       <c r="I7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="8">
         <v>44536</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="s">
@@ -771,18 +733,18 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="8">
         <v>44537</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="23" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I9" t="s">
@@ -790,79 +752,79 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>44538</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="24"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="12"/>
       <c r="I10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="8">
         <v>44539</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="24"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="12"/>
       <c r="I11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
+      <c r="B12" s="8">
         <v>44540</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="25"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="13"/>
       <c r="I12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
+      <c r="B13" s="8">
         <v>44541</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="6"/>
       <c r="I13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="12">
+      <c r="B14" s="8">
         <v>44542</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="9"/>
       <c r="I14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+      <c r="B15" s="8">
         <v>44543</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="9" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I15" t="s">
@@ -870,72 +832,72 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+      <c r="B16" s="8">
         <v>44544</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="13"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
+      <c r="B17" s="8">
         <v>44545</v>
       </c>
       <c r="C17" s="15"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
+      <c r="B18" s="8">
         <v>44546</v>
       </c>
       <c r="C18" s="15"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+      <c r="B19" s="8">
         <v>44547</v>
       </c>
       <c r="C19" s="15"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="5"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
+      <c r="B20" s="8">
         <v>44548</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="6" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+      <c r="B21" s="8">
         <v>44549</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -955,18 +917,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1153,14 +1115,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E70EDAD-331A-46C8-9CBE-243B28A6A96D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1028B10C-001E-4A2B-8DAC-FE067E1C860E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1173,6 +1127,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E70EDAD-331A-46C8-9CBE-243B28A6A96D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
230710 - BLTAnh - New resources
</commit_message>
<xml_diff>
--- a/Docs/Timeline.xlsx
+++ b/Docs/Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SoftEng\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/19120163_student_hcmus_edu_vn/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C65C7AA-1399-448E-A6B8-F6ECB2CD68EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{8249A737-0AAB-4BFA-B6B2-5FB40B02FF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CA78461-22C6-4C47-B2A7-EF827C0DB303}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -841,9 +841,9 @@
       <c r="D16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
@@ -851,9 +851,9 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
@@ -861,9 +861,9 @@
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
@@ -871,9 +871,9 @@
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
@@ -881,8 +881,8 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="5" t="s">
         <v>27</v>
       </c>
@@ -917,12 +917,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -931,7 +925,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100182A0FD1201485479895ED3ABF5F8B85" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="079ee4fb2fabb65520d6a613be97d116">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7b495183-be68-46b6-9f93-303bb4369acc" xmlns:ns4="e8900967-fe10-44ee-8cdd-dcc614f4f1dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="352e32c72f0a7a307122e470dfb98c00" ns3:_="" ns4:_="">
     <xsd:import namespace="7b495183-be68-46b6-9f93-303bb4369acc"/>
@@ -1114,24 +1108,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1028B10C-001E-4A2B-8DAC-FE067E1C860E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="e8900967-fe10-44ee-8cdd-dcc614f4f1dd"/>
-    <ds:schemaRef ds:uri="7b495183-be68-46b6-9f93-303bb4369acc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E70EDAD-331A-46C8-9CBE-243B28A6A96D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1139,7 +1122,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E09C09F-8B5A-4369-9A12-6EC610C2EE49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1156,4 +1139,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1028B10C-001E-4A2B-8DAC-FE067E1C860E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7b495183-be68-46b6-9f93-303bb4369acc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e8900967-fe10-44ee-8cdd-dcc614f4f1dd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>